<commit_message>
looks like somebody added plugins
</commit_message>
<xml_diff>
--- a/scraper/top_remaining_spreadsheets_states/top_remaining_AR.xlsx
+++ b/scraper/top_remaining_spreadsheets_states/top_remaining_AR.xlsx
@@ -44,7 +44,7 @@
     <t>3 Times Lucky</t>
   </si>
   <si>
-    <t>2019-03-07</t>
+    <t>2019-03-12</t>
   </si>
   <si>
     <t>Cash on the Spot</t>
@@ -56,21 +56,21 @@
     <t>Wild 10's</t>
   </si>
   <si>
+    <t>BETTY BOOP™</t>
+  </si>
+  <si>
+    <t>Hit $100!</t>
+  </si>
+  <si>
+    <t>Super 7's</t>
+  </si>
+  <si>
     <t>10X Payout</t>
   </si>
   <si>
-    <t>Hit $100!</t>
-  </si>
-  <si>
-    <t>BETTY BOOP™</t>
-  </si>
-  <si>
     <t>Cash $100's</t>
   </si>
   <si>
-    <t>Super 7's</t>
-  </si>
-  <si>
     <t>Fast $100</t>
   </si>
   <si>
@@ -104,12 +104,12 @@
     <t>Lady Jumbo Bucks</t>
   </si>
   <si>
+    <t>Jumbo Bucks</t>
+  </si>
+  <si>
     <t>20X The Money</t>
   </si>
   <si>
-    <t>Jumbo Bucks</t>
-  </si>
-  <si>
     <t>$20,000 Money Bag</t>
   </si>
   <si>
@@ -173,21 +173,21 @@
     <t>25X</t>
   </si>
   <si>
+    <t>50X Payout</t>
+  </si>
+  <si>
     <t>Cash Multiplier</t>
   </si>
   <si>
     <t>Stacks of Cash</t>
   </si>
   <si>
-    <t>50X Payout</t>
+    <t>$100,000 Triple Win</t>
   </si>
   <si>
     <t>Hit $500!</t>
   </si>
   <si>
-    <t>$100,000 Triple Win</t>
-  </si>
-  <si>
     <t>Win $500!</t>
   </si>
   <si>
@@ -206,30 +206,30 @@
     <t>Bonus Payout</t>
   </si>
   <si>
+    <t>$250,000 Riches</t>
+  </si>
+  <si>
     <t>$200,000 Jackpot</t>
   </si>
   <si>
-    <t>$250,000 Riches</t>
-  </si>
-  <si>
     <t>Gigantic Jumbo Bucks</t>
   </si>
   <si>
+    <t>$200,000 Bonus</t>
+  </si>
+  <si>
     <t>Big Multiplier</t>
   </si>
   <si>
-    <t>$200,000 Bonus</t>
-  </si>
-  <si>
     <t>$200,000 Cash Vault HD</t>
   </si>
   <si>
+    <t>100X Payout</t>
+  </si>
+  <si>
     <t>Cash $1000's</t>
   </si>
   <si>
-    <t>100X Payout</t>
-  </si>
-  <si>
     <t>Hit $5,000!</t>
   </si>
   <si>
@@ -260,10 +260,10 @@
     <t>Ultimate Millions</t>
   </si>
   <si>
+    <t>$50K Blowout</t>
+  </si>
+  <si>
     <t>200X Payout</t>
-  </si>
-  <si>
-    <t>$50K Blowout</t>
   </si>
 </sst>
 </file>
@@ -721,10 +721,10 @@
         <v>13</v>
       </c>
       <c r="D6">
-        <v>490</v>
+        <v>471</v>
       </c>
       <c r="E6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
@@ -744,7 +744,7 @@
         <v>481</v>
       </c>
       <c r="E7">
-        <v>2046</v>
+        <v>1972</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
@@ -761,10 +761,10 @@
         <v>15</v>
       </c>
       <c r="D8">
-        <v>471</v>
+        <v>485</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F8" t="s">
         <v>9</v>
@@ -781,10 +781,10 @@
         <v>16</v>
       </c>
       <c r="D9">
-        <v>425</v>
+        <v>490</v>
       </c>
       <c r="E9">
-        <v>813</v>
+        <v>4</v>
       </c>
       <c r="F9" t="s">
         <v>9</v>
@@ -801,10 +801,10 @@
         <v>17</v>
       </c>
       <c r="D10">
-        <v>485</v>
+        <v>425</v>
       </c>
       <c r="E10">
-        <v>3</v>
+        <v>813</v>
       </c>
       <c r="F10" t="s">
         <v>9</v>
@@ -824,7 +824,7 @@
         <v>453</v>
       </c>
       <c r="E11">
-        <v>780</v>
+        <v>767</v>
       </c>
       <c r="F11" t="s">
         <v>9</v>
@@ -1021,10 +1021,10 @@
         <v>29</v>
       </c>
       <c r="D21">
-        <v>435</v>
+        <v>486</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F21" t="s">
         <v>9</v>
@@ -1041,10 +1041,10 @@
         <v>30</v>
       </c>
       <c r="D22">
-        <v>486</v>
+        <v>435</v>
       </c>
       <c r="E22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F22" t="s">
         <v>9</v>
@@ -1124,7 +1124,7 @@
         <v>482</v>
       </c>
       <c r="E26">
-        <v>1308</v>
+        <v>1251</v>
       </c>
       <c r="F26" t="s">
         <v>9</v>
@@ -1164,7 +1164,7 @@
         <v>454</v>
       </c>
       <c r="E28">
-        <v>947</v>
+        <v>936</v>
       </c>
       <c r="F28" t="s">
         <v>9</v>
@@ -1441,10 +1441,10 @@
         <v>52</v>
       </c>
       <c r="D42">
-        <v>478</v>
+        <v>492</v>
       </c>
       <c r="E42">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F42" t="s">
         <v>9</v>
@@ -1461,10 +1461,10 @@
         <v>53</v>
       </c>
       <c r="D43">
-        <v>465</v>
+        <v>478</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F43" t="s">
         <v>9</v>
@@ -1481,10 +1481,10 @@
         <v>54</v>
       </c>
       <c r="D44">
-        <v>492</v>
+        <v>465</v>
       </c>
       <c r="E44">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F44" t="s">
         <v>9</v>
@@ -1501,10 +1501,10 @@
         <v>55</v>
       </c>
       <c r="D45">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="E45">
-        <v>1911</v>
+        <v>1</v>
       </c>
       <c r="F45" t="s">
         <v>9</v>
@@ -1521,10 +1521,10 @@
         <v>56</v>
       </c>
       <c r="D46">
-        <v>474</v>
+        <v>483</v>
       </c>
       <c r="E46">
-        <v>1</v>
+        <v>1781</v>
       </c>
       <c r="F46" t="s">
         <v>9</v>
@@ -1641,7 +1641,7 @@
         <v>63</v>
       </c>
       <c r="D52">
-        <v>447</v>
+        <v>466</v>
       </c>
       <c r="E52">
         <v>1</v>
@@ -1661,7 +1661,7 @@
         <v>64</v>
       </c>
       <c r="D53">
-        <v>466</v>
+        <v>447</v>
       </c>
       <c r="E53">
         <v>1</v>
@@ -1701,10 +1701,10 @@
         <v>66</v>
       </c>
       <c r="D55">
-        <v>470</v>
+        <v>489</v>
       </c>
       <c r="E55">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F55" t="s">
         <v>9</v>
@@ -1721,10 +1721,10 @@
         <v>67</v>
       </c>
       <c r="D56">
-        <v>489</v>
+        <v>470</v>
       </c>
       <c r="E56">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="s">
         <v>9</v>
@@ -1761,10 +1761,10 @@
         <v>69</v>
       </c>
       <c r="D58">
-        <v>428</v>
+        <v>493</v>
       </c>
       <c r="E58">
-        <v>61</v>
+        <v>4</v>
       </c>
       <c r="F58" t="s">
         <v>9</v>
@@ -1781,10 +1781,10 @@
         <v>70</v>
       </c>
       <c r="D59">
-        <v>493</v>
+        <v>428</v>
       </c>
       <c r="E59">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="F59" t="s">
         <v>9</v>
@@ -1804,7 +1804,7 @@
         <v>484</v>
       </c>
       <c r="E60">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="F60" t="s">
         <v>9</v>
@@ -1844,7 +1844,7 @@
         <v>479</v>
       </c>
       <c r="E62">
-        <v>935</v>
+        <v>819</v>
       </c>
       <c r="F62" t="s">
         <v>9</v>
@@ -1981,10 +1981,10 @@
         <v>81</v>
       </c>
       <c r="D69">
-        <v>494</v>
+        <v>461</v>
       </c>
       <c r="E69">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="F69" t="s">
         <v>9</v>
@@ -2001,10 +2001,10 @@
         <v>82</v>
       </c>
       <c r="D70">
-        <v>461</v>
+        <v>494</v>
       </c>
       <c r="E70">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="F70" t="s">
         <v>9</v>

</xml_diff>